<commit_message>
added 'created_at_field' to metadata docs
</commit_message>
<xml_diff>
--- a/dbt_project_setup_automation/ip/data_src_a_data_dictionary.xlsx
+++ b/dbt_project_setup_automation/ip/data_src_a_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulfry/Dropbox/tech/code/git-repos/dbt_repos/dbt/dbt_project_setup_automation/ip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15238725-30C4-0943-86AB-7EBA69098561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192028DF-C963-C844-9B76-40A49DBC865B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="8660" windowWidth="28800" windowHeight="17500" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
   </bookViews>
   <sheets>
     <sheet name="data_src_a_table_a" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="26">
   <si>
     <t>accepted_values</t>
   </si>
@@ -102,13 +102,16 @@
     <t>primary_key</t>
   </si>
   <si>
-    <t>loaded_at_field</t>
-  </si>
-  <si>
     <t>unique</t>
   </si>
   <si>
     <t>not_null</t>
+  </si>
+  <si>
+    <t>created_at_field</t>
+  </si>
+  <si>
+    <t>updated_at_field</t>
   </si>
 </sst>
 </file>
@@ -204,15 +207,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}" name="Table2" displayName="Table2" ref="B3:M7" totalsRowShown="0">
-  <autoFilter ref="B3:M7" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}" name="Table2" displayName="Table2" ref="B3:N7" totalsRowShown="0">
+  <autoFilter ref="B3:N7" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{72D067D0-8E61-8546-B65D-7F7FF631A866}" name="no"/>
     <tableColumn id="2" xr3:uid="{DB1DC045-AFC3-DF49-AC9B-4C31084BA7B9}" name="table"/>
     <tableColumn id="3" xr3:uid="{5CDBA1C4-4CF5-CD45-9FBF-36494DEC28CB}" name="field"/>
     <tableColumn id="4" xr3:uid="{A8218E91-E332-DA4B-ACDC-0F4DC4066661}" name="description" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{99E77446-E85F-5E42-A8ED-3E8C7105A15C}" name="primary_key"/>
-    <tableColumn id="12" xr3:uid="{B2726D3A-32BD-504C-8271-90C72AC2A7AA}" name="loaded_at_field"/>
+    <tableColumn id="12" xr3:uid="{B2726D3A-32BD-504C-8271-90C72AC2A7AA}" name="created_at_field"/>
+    <tableColumn id="13" xr3:uid="{9F4078F1-34F1-374E-BF8D-38F428EAB147}" name="updated_at_field"/>
     <tableColumn id="11" xr3:uid="{20AE297A-49F0-164A-831E-045BFB42ED03}" name="unique"/>
     <tableColumn id="6" xr3:uid="{49C67C95-EF85-EA42-A1AE-7B17EA605A4B}" name="not_null"/>
     <tableColumn id="7" xr3:uid="{26664B8F-5D74-0642-9DF6-0B6BD53CA600}" name="accepted_values"/>
@@ -225,15 +229,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4B325D8-FB0F-0342-964F-517F4E3F298B}" name="Table24" displayName="Table24" ref="B3:M6" totalsRowShown="0">
-  <autoFilter ref="B3:M6" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4B325D8-FB0F-0342-964F-517F4E3F298B}" name="Table24" displayName="Table24" ref="B3:N6" totalsRowShown="0">
+  <autoFilter ref="B3:N6" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{7CF1B6FB-CEBC-B54B-9E7A-3BE1AE2E3C17}" name="no"/>
     <tableColumn id="2" xr3:uid="{22A6305B-EF5E-4541-BAB2-7901F6582337}" name="table"/>
     <tableColumn id="3" xr3:uid="{F87EAFF0-4ABE-0F46-8960-20A0CC25DFB5}" name="field"/>
     <tableColumn id="4" xr3:uid="{F31B5585-9664-F84A-992C-D5C070BB7E59}" name="description" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{155A533D-B2FE-8E43-A8BA-0B846864184F}" name="primary_key"/>
-    <tableColumn id="6" xr3:uid="{F509BE04-279E-8D41-8C71-9109656824F4}" name="loaded_at_field"/>
+    <tableColumn id="13" xr3:uid="{AFE38834-2C77-F54C-81E6-B82AFC3D9929}" name="created_at_field"/>
+    <tableColumn id="6" xr3:uid="{F509BE04-279E-8D41-8C71-9109656824F4}" name="updated_at_field"/>
     <tableColumn id="12" xr3:uid="{BD592517-EC8E-A64B-9BC8-9774AB54B774}" name="unique"/>
     <tableColumn id="11" xr3:uid="{BFC6A842-B687-9E42-BC6E-BBAC76B8848F}" name="not_null"/>
     <tableColumn id="7" xr3:uid="{13995F2A-884C-EC4C-91AE-A78AA7FC7811}" name="accepted_values"/>
@@ -542,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A3F06E-3DE3-9748-8162-6D49E20586D1}">
-  <dimension ref="B2:M7"/>
+  <dimension ref="B2:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,16 +560,17 @@
     <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
@@ -589,8 +595,11 @@
       <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -607,28 +616,31 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -644,14 +656,14 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -664,11 +676,11 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -681,11 +693,11 @@
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" ht="34" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -698,10 +710,10 @@
       <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>11</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -715,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E301CF-5EFF-2C41-B661-9A4150B69AC2}">
-  <dimension ref="B2:M6"/>
+  <dimension ref="B2:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,15 +740,16 @@
     <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
@@ -761,8 +774,11 @@
       <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -779,28 +795,31 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -816,14 +835,14 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -836,11 +855,11 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -853,13 +872,13 @@
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>